<commit_message>
added pdf of results
</commit_message>
<xml_diff>
--- a/Performance-Evaluation/Results.xlsx
+++ b/Performance-Evaluation/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BE8EA132-78A1-4909-B419-EE32FF2EB710}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{78880D7A-6725-4EF6-843F-0A2A869FAFAB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22722,8 +22722,8 @@
       <xdr:rowOff>100614</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>373601</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>523042</xdr:colOff>
       <xdr:row>130</xdr:row>
       <xdr:rowOff>69542</xdr:rowOff>
     </xdr:to>
@@ -23162,8 +23162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="103" workbookViewId="0">
-      <selection activeCell="L154" sqref="L154"/>
+    <sheetView tabSelected="1" topLeftCell="L17" zoomScale="103" workbookViewId="0">
+      <selection activeCell="AD115" sqref="AD115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23918,6 +23918,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E29:G29"/>
@@ -23932,12 +23938,6 @@
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>